<commit_message>
Raport z testów: wykresy.
</commit_message>
<xml_diff>
--- a/doc/RaportZTestow/F_0.25_Cr_0.25_L_5.xlsx
+++ b/doc/RaportZTestow/F_0.25_Cr_0.25_L_5.xlsx
@@ -605,21 +605,6 @@
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -652,6 +637,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,6 +659,396 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Expected</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>-1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-900</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Our</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>-1384.1826876294408</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1156.7281775407146</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1805624.7927669925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-179.02725433401883</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-970.73637864046771</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-899.90382303651995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-794.18565887154773</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-679.97658135969198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-597.88570059677807</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-496.87774684185018</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-396.77795620779267</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-292.82959578134023</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-192.94305317378578</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-67.190516219761321</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>210.36352872829093</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200.47072696862452</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>306.77848671986027</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>408.95783165433198</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>500.63589752293615</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>600.31337766247668</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>844.51566645913647</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1044.9889835198107</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1151.5288705979447</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1037.0146736513038</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1207.8373692720236</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1221.5438889893928</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1645.2269142658727</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1711.4529004271042</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Classic</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>-1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4641.8598781362653</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1190.8149128190776</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-887.02179062491416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-999.99999999999932</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-899.69250671958616</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-799.95260331825534</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-684.68446548167367</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-598.79041319303781</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-499.8907845812505</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-399.99999999993901</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-297.54007090388103</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-197.30946493271395</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-99.935394363805244</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>261.8744023833035</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200.54151981899196</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>305.0946196124973</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>407.83088863098226</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>500.06368882485918</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>600.41355647209571</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>801.86140056446709</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>829.7369355788752</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1224.0467555144432</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1040.0080257988225</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1202.3976429911438</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1285.9266942711251</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1609.652473298554</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1666.2656028451881</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="102448512"/>
+        <c:axId val="102471552"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="102448512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102471552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="102471552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102448512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -948,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -959,1362 +1349,1362 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickTop="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="35"/>
+      <c r="E1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="37"/>
+      <c r="K1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="35"/>
+      <c r="M1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="6"/>
+      <c r="N1" s="38"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="21" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="8">
         <v>-1400</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="9">
         <f>G3</f>
         <v>-1384.1826876294408</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="10">
         <f>H3</f>
         <v>-1400</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="11">
         <v>-1333.31011354203</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="8">
         <v>-1400</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="9">
         <v>-1384.1826876294408</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="10">
         <v>-1400</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="11">
         <v>-1370.2512526145422</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="8">
         <v>-1400</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="9">
         <v>-1367.3531996732579</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="10">
         <v>-1400</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="11">
         <v>15.016513515480243</v>
       </c>
-      <c r="N3" s="17">
+      <c r="N3" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="23">
         <v>-1300</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="24">
         <f t="shared" ref="C4:C30" si="0">G4</f>
         <v>1156.7281775407146</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="25">
         <f t="shared" ref="D4:D30" si="1">H4</f>
         <v>4641.8598781362653</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="26">
         <v>30107.534983490055</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="23">
         <v>56645.84394786015</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="24">
         <v>1156.7281775407146</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="25">
         <v>4641.8598781362653</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="26">
         <v>13810.683308032103</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="23">
         <v>14740.683208539995</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="24">
         <v>14887.493209405711</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="25">
         <v>21565.067775685566</v>
       </c>
-      <c r="M4" s="31">
+      <c r="M4" s="26">
         <v>9928.9770171142009</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="27">
         <v>17062.732594929737</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="4">
         <v>-1200</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="6">
         <f t="shared" si="0"/>
         <v>1805624.7927669925</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="7">
         <f t="shared" si="1"/>
         <v>-1190.8149128190776</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="5">
         <v>30634900.758200429</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="4">
         <v>-1161.1861427213175</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="6">
         <v>1805624.7927669925</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="7">
         <v>-1190.8149128190776</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="5">
         <v>10470177.137248093</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="4">
         <v>-1186.2212311698395</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="6">
         <v>13080637.750825349</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="7">
         <v>-1183.4015652952301</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="5">
         <v>10998503.861660568</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="3">
         <v>8.7240857528089286</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="23">
         <v>-1100</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="24">
         <f t="shared" si="0"/>
         <v>-179.02725433401883</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="25">
         <f t="shared" si="1"/>
         <v>-887.02179062491416</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="26">
         <v>4096.4630913859655</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="23">
         <v>2511.9692956915237</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="24">
         <v>-179.02725433401883</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="25">
         <v>-887.02179062491416</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="26">
         <v>1183.8407012906364</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="23">
         <v>163.8953145550297</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="24">
         <v>1307.5641767270756</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="25">
         <v>462.16362123654687</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="26">
         <v>1278.7903222557591</v>
       </c>
-      <c r="N6" s="32">
+      <c r="N6" s="27">
         <v>1090.9669874081244</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="4">
         <v>-1000</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>-970.73637864046771</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="7">
         <f t="shared" si="1"/>
         <v>-999.99999999999932</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="5">
         <v>-925.91408494127677</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="4">
         <v>-999.99999999999625</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="6">
         <v>-970.73637864046771</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="7">
         <v>-999.99999999999932</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="5">
         <v>-953.68118909428813</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="4">
         <v>-999.99999999999795</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="6">
         <v>-951.84257774437208</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="7">
         <v>-999.99999999999784</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="5">
         <v>16.208610852701494</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="3">
         <v>1.0658035770291185E-12</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="23">
         <v>-900</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="24">
         <f t="shared" si="0"/>
         <v>-899.90382303651995</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="25">
         <f t="shared" si="1"/>
         <v>-899.69250671958616</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="26">
         <v>-893.6091023777617</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="23">
         <v>-898.23984275993382</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="24">
         <v>-899.90382303651995</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="25">
         <v>-899.69250671958616</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="26">
         <v>-899.38356668668985</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="23">
         <v>-899.19442639750446</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K8" s="24">
         <v>-898.4350124272645</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="25">
         <v>-899.12519702772556</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="26">
         <v>1.9557957998402173</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="27">
         <v>0.45692089294119392</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="4">
         <v>-800</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="6">
         <f t="shared" si="0"/>
         <v>-794.18565887154773</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="7">
         <f t="shared" si="1"/>
         <v>-799.95260331825534</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="5">
         <v>-785.07542528354577</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="4">
         <v>-799.89513214045735</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="6">
         <v>-794.18565887154773</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="7">
         <v>-799.95260331825534</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="5">
         <v>-790.4025408977468</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="4">
         <v>-799.93934627313229</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="6">
         <v>-789.95164470370037</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="7">
         <v>-799.93203077272358</v>
       </c>
-      <c r="M9" s="10">
+      <c r="M9" s="5">
         <v>2.8575848774486903</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="3">
         <v>2.1418827726540548E-2</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="23">
         <v>-700</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="24">
         <f t="shared" si="0"/>
         <v>-679.97658135969198</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="25">
         <f t="shared" si="1"/>
         <v>-684.68446548167367</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="26">
         <v>-679.88899092191423</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="23">
         <v>-679.9081673730276</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="24">
         <v>-679.97658135969198</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="25">
         <v>-684.68446548167367</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="26">
         <v>-679.91987371346772</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="23">
         <v>-681.66026358975409</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="24">
         <v>-679.92472477213812</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="25">
         <v>-682.02229743322289</v>
       </c>
-      <c r="M10" s="31">
+      <c r="M10" s="26">
         <v>2.6809981919948142E-2</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="27">
         <v>2.0766320701113128</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="4">
         <v>-600</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="6">
         <f t="shared" si="0"/>
         <v>-597.88570059677807</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="7">
         <f t="shared" si="1"/>
         <v>-598.79041319303781</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="5">
         <v>-597.35454674315235</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="4">
         <v>-597.93546012862464</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="6">
         <v>-597.88570059677807</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="7">
         <v>-598.79041319303781</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="5">
         <v>-597.67182740381418</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="4">
         <v>-598.50117329554791</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="6">
         <v>-597.65693468385155</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="7">
         <v>-598.43308721246251</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="5">
         <v>0.20039624432895289</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="3">
         <v>0.24313420574419253</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="23">
         <v>-500</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="24">
         <f t="shared" si="0"/>
         <v>-496.87774684185018</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="25">
         <f t="shared" si="1"/>
         <v>-499.8907845812505</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="26">
         <v>-482.50444995381235</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="23">
         <v>-499.68650997440773</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="24">
         <v>-496.87774684185018</v>
       </c>
-      <c r="H12" s="30">
+      <c r="H12" s="25">
         <v>-499.8907845812505</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="26">
         <v>-492.86071024378873</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="23">
         <v>-499.7615878538287</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12" s="24">
         <v>-491.76533207143541</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="25">
         <v>-499.78197518663688</v>
       </c>
-      <c r="M12" s="31">
+      <c r="M12" s="26">
         <v>4.6124095749285452</v>
       </c>
-      <c r="N12" s="32">
+      <c r="N12" s="27">
         <v>6.2524730837668935E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="4">
         <v>-400</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="6">
         <f t="shared" si="0"/>
         <v>-396.77795620779267</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="7">
         <f t="shared" si="1"/>
         <v>-399.99999999993901</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="5">
         <v>-385.09267383358599</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="4">
         <v>-399.99999999573748</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="6">
         <v>-396.77795620779267</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="7">
         <v>-399.99999999993901</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="5">
         <v>-392.29766145862527</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="4">
         <v>-399.99999999963427</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="6">
         <v>-391.70885967337881</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="7">
         <v>-399.99999999929628</v>
       </c>
-      <c r="M13" s="10">
+      <c r="M13" s="5">
         <v>3.4867244863161928</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="3">
         <v>1.2644947682896401E-9</v>
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="23">
         <v>-300</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="24">
         <f t="shared" si="0"/>
         <v>-292.82959578134023</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="25">
         <f t="shared" si="1"/>
         <v>-297.54007090388103</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="26">
         <v>-288.87962515879354</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="23">
         <v>-293.93755632445334</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="24">
         <v>-292.82959578134023</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="25">
         <v>-297.54007090388103</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="26">
         <v>-291.62087545783123</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="23">
         <v>-295.77970712206957</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="24">
         <v>-291.54589292389181</v>
       </c>
-      <c r="L14" s="30">
+      <c r="L14" s="25">
         <v>-295.88147366650418</v>
       </c>
-      <c r="M14" s="31">
+      <c r="M14" s="26">
         <v>1.2090895012031766</v>
       </c>
-      <c r="N14" s="32">
+      <c r="N14" s="27">
         <v>1.2177658014516648</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="4">
         <v>-200</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="6">
         <f t="shared" si="0"/>
         <v>-192.94305317378578</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="7">
         <f t="shared" si="1"/>
         <v>-197.30946493271395</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="5">
         <v>-184.22839666629562</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="4">
         <v>-194.15311235070493</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="6">
         <v>-192.94305317378578</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="7">
         <v>-197.30946493271395</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="5">
         <v>-187.26439031801175</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="4">
         <v>-196.42114652634689</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="6">
         <v>-187.85640373520926</v>
       </c>
-      <c r="L15" s="12">
+      <c r="L15" s="7">
         <v>-196.15400281705757</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="5">
         <v>3.0262319591094666</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="3">
         <v>1.0819735049330443</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="23">
         <v>-100</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="24">
         <f t="shared" si="0"/>
         <v>-67.190516219761321</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="25">
         <f t="shared" si="1"/>
         <v>-99.935394363805244</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="26">
         <v>51.848436567842327</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="23">
         <v>-99.274371161579438</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="24">
         <v>-67.190516219761321</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="25">
         <v>-99.935394363805244</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="26">
         <v>-6.4508481110764251</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="23">
         <v>-99.796194226051512</v>
       </c>
-      <c r="K16" s="29">
+      <c r="K16" s="24">
         <v>-3.8654861767074409</v>
       </c>
-      <c r="L16" s="30">
+      <c r="L16" s="25">
         <v>-99.735296525588325</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M16" s="26">
         <v>36.272597533440475</v>
       </c>
-      <c r="N16" s="32">
+      <c r="N16" s="27">
         <v>0.19681854706706975</v>
       </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="4">
         <v>100</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="6">
         <f t="shared" si="0"/>
         <v>210.36352872829093</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="7">
         <f t="shared" si="1"/>
         <v>261.8744023833035</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="5">
         <v>446.37896567165831</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="4">
         <v>432.34953951315401</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="6">
         <v>210.36352872829093</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="7">
         <v>261.8744023833035</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="5">
         <v>290.88007772503227</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="4">
         <v>324.23689564838173</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="6">
         <v>301.31617452343994</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="7">
         <v>329.65429224365715</v>
       </c>
-      <c r="M17" s="10">
+      <c r="M17" s="5">
         <v>73.569015822240416</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="3">
         <v>59.756282949591828</v>
       </c>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="23">
         <v>200</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="24">
         <f t="shared" si="0"/>
         <v>200.47072696862452</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="25">
         <f t="shared" si="1"/>
         <v>200.54151981899196</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="26">
         <v>201.02533210644549</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="23">
         <v>201.29055468229328</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="24">
         <v>200.47072696862452</v>
       </c>
-      <c r="H18" s="30">
+      <c r="H18" s="25">
         <v>200.54151981899196</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="26">
         <v>200.77231368772814</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="23">
         <v>200.89418437519555</v>
       </c>
-      <c r="K18" s="29">
+      <c r="K18" s="24">
         <v>200.7899794788276</v>
       </c>
-      <c r="L18" s="30">
+      <c r="L18" s="25">
         <v>200.89270928458546</v>
       </c>
-      <c r="M18" s="31">
+      <c r="M18" s="26">
         <v>0.16452292277933259</v>
       </c>
-      <c r="N18" s="32">
+      <c r="N18" s="27">
         <v>0.20874488815022407</v>
       </c>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="4">
         <v>300</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="6">
         <f t="shared" si="0"/>
         <v>306.77848671986027</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="7">
         <f t="shared" si="1"/>
         <v>305.0946196124973</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="5">
         <v>312.09469506567569</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="4">
         <v>305.53264539562082</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="6">
         <v>306.77848671986027</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="7">
         <v>305.0946196124973</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="5">
         <v>309.43502297650519</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="4">
         <v>305.27357053894457</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="6">
         <v>309.38591178318376</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="7">
         <v>305.28145733884065</v>
       </c>
-      <c r="M19" s="10">
+      <c r="M19" s="5">
         <v>1.6668950176618205</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="3">
         <v>0.13165115584143472</v>
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="23">
         <v>400</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C20" s="24">
         <f t="shared" si="0"/>
         <v>408.95783165433198</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="25">
         <f t="shared" si="1"/>
         <v>407.83088863098226</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="26">
         <v>415.99455731756524</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="23">
         <v>411.1644489124771</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="24">
         <v>408.95783165433198</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="25">
         <v>407.83088863098226</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="26">
         <v>413.20981913116441</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J20" s="23">
         <v>409.07634399156518</v>
       </c>
-      <c r="K20" s="29">
+      <c r="K20" s="24">
         <v>412.9012159086522</v>
       </c>
-      <c r="L20" s="30">
+      <c r="L20" s="25">
         <v>409.4511980062307</v>
       </c>
-      <c r="M20" s="31">
+      <c r="M20" s="26">
         <v>1.8034542267493907</v>
       </c>
-      <c r="N20" s="32">
+      <c r="N20" s="27">
         <v>1.3515672440353308</v>
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="4">
         <v>500</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="6">
         <f t="shared" si="0"/>
         <v>500.63589752293615</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="7">
         <f t="shared" si="1"/>
         <v>500.06368882485918</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="5">
         <v>505.62570905598926</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="4">
         <v>500.24724057055744</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="6">
         <v>500.63589752293615</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="7">
         <v>500.06368882485918</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="5">
         <v>501.94578898217105</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="4">
         <v>500.13745252821269</v>
       </c>
-      <c r="K21" s="11">
+      <c r="K21" s="6">
         <v>502.1029959386305</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="7">
         <v>500.15505306535329</v>
       </c>
-      <c r="M21" s="10">
+      <c r="M21" s="5">
         <v>1.4421064859973953</v>
       </c>
-      <c r="N21" s="8">
+      <c r="N21" s="3">
         <v>6.5074777337296524E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="23">
         <v>600</v>
       </c>
-      <c r="C22" s="29">
+      <c r="C22" s="24">
         <f t="shared" si="0"/>
         <v>600.31337766247668</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="25">
         <f t="shared" si="1"/>
         <v>600.41355647209571</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="26">
         <v>601.03941043254076</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="23">
         <v>600.87343728363203</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="24">
         <v>600.31337766247668</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="25">
         <v>600.41355647209571</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="26">
         <v>600.60323384539242</v>
       </c>
-      <c r="J22" s="28">
+      <c r="J22" s="23">
         <v>600.55298361381961</v>
       </c>
-      <c r="K22" s="29">
+      <c r="K22" s="24">
         <v>600.67346091590514</v>
       </c>
-      <c r="L22" s="30">
+      <c r="L22" s="25">
         <v>600.61665548746294</v>
       </c>
-      <c r="M22" s="31">
+      <c r="M22" s="26">
         <v>0.26963853287937173</v>
       </c>
-      <c r="N22" s="32">
+      <c r="N22" s="27">
         <v>0.18462026695406084</v>
       </c>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="4">
         <v>700</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="6">
         <f t="shared" si="0"/>
         <v>844.51566645913647</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="7">
         <f t="shared" si="1"/>
         <v>801.86140056446709</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="5">
         <v>1030.7446841759449</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="4">
         <v>960.60344254360189</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="6">
         <v>844.51566645913647</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="7">
         <v>801.86140056446709</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="5">
         <v>1022.9325258823761</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="4">
         <v>812.78649024089384</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="6">
         <v>989.75260158185267</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="7">
         <v>844.07376337959715</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="5">
         <v>73.521230713976834</v>
       </c>
-      <c r="N23" s="8">
+      <c r="N23" s="3">
         <v>56.328386999836567</v>
       </c>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="23">
         <v>800</v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24" s="24">
         <f t="shared" si="0"/>
         <v>1044.9889835198107</v>
       </c>
-      <c r="D24" s="30">
+      <c r="D24" s="25">
         <f t="shared" si="1"/>
         <v>829.7369355788752</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="26">
         <v>1278.0414939252203</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="23">
         <v>972.81277216461228</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="24">
         <v>1044.9889835198107</v>
       </c>
-      <c r="H24" s="30">
+      <c r="H24" s="25">
         <v>829.7369355788752</v>
       </c>
-      <c r="I24" s="31">
+      <c r="I24" s="26">
         <v>1200.2681502668283</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="23">
         <v>937.00224263479322</v>
       </c>
-      <c r="K24" s="29">
+      <c r="K24" s="24">
         <v>1179.9393902812276</v>
       </c>
-      <c r="L24" s="30">
+      <c r="L24" s="25">
         <v>930.24205360507301</v>
       </c>
-      <c r="M24" s="31">
+      <c r="M24" s="26">
         <v>87.217536696158987</v>
       </c>
-      <c r="N24" s="32">
+      <c r="N24" s="27">
         <v>38.802394576959479</v>
       </c>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="4">
         <v>900</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="6">
         <f t="shared" si="0"/>
         <v>1151.5288705979447</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="7">
         <f t="shared" si="1"/>
         <v>1224.0467555144432</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="5">
         <v>1509.5445803438179</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="4">
         <v>1500.4086197983834</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="6">
         <v>1151.5288705979447</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="7">
         <v>1224.0467555144432</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="5">
         <v>1390.3603727040074</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="4">
         <v>1397.0196985153771</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="6">
         <v>1357.2990470290788</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="7">
         <v>1375.1781028337648</v>
       </c>
-      <c r="M25" s="10">
+      <c r="M25" s="5">
         <v>113.81768339914758</v>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="3">
         <v>92.976928716038174</v>
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="23">
         <v>1000</v>
       </c>
-      <c r="C26" s="29">
+      <c r="C26" s="24">
         <f t="shared" si="0"/>
         <v>1037.0146736513038</v>
       </c>
-      <c r="D26" s="30">
+      <c r="D26" s="25">
         <f t="shared" si="1"/>
         <v>1040.0080257988225</v>
       </c>
-      <c r="E26" s="31">
+      <c r="E26" s="26">
         <v>1120.7864467697552</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="23">
         <v>1123.718358793592</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="24">
         <v>1037.0146736513038</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="25">
         <v>1040.0080257988225</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="26">
         <v>1096.2085806003697</v>
       </c>
-      <c r="J26" s="28">
+      <c r="J26" s="23">
         <v>1115.3686496485052</v>
       </c>
-      <c r="K26" s="29">
+      <c r="K26" s="24">
         <v>1088.3774856305547</v>
       </c>
-      <c r="L26" s="30">
+      <c r="L26" s="25">
         <v>1107.6566756763259</v>
       </c>
-      <c r="M26" s="31">
+      <c r="M26" s="26">
         <v>26.412107563586929</v>
       </c>
-      <c r="N26" s="32">
+      <c r="N26" s="27">
         <v>24.692802921795455</v>
       </c>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="4">
         <v>1100</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="6">
         <f t="shared" si="0"/>
         <v>1207.8373692720236</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="7">
         <f t="shared" si="1"/>
         <v>1202.3976429911438</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="5">
         <v>1238.8293477572572</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="4">
         <v>1209.0364323468827</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="6">
         <v>1207.8373692720236</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="7">
         <v>1202.3976429911438</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="5">
         <v>1227.0376745703202</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="4">
         <v>1206.578046091628</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="6">
         <v>1226.7835308184426</v>
       </c>
-      <c r="L27" s="12">
+      <c r="L27" s="7">
         <v>1206.5505589493901</v>
       </c>
-      <c r="M27" s="10">
+      <c r="M27" s="5">
         <v>8.914443417158564</v>
       </c>
-      <c r="N27" s="8">
+      <c r="N27" s="3">
         <v>2.0220865267793524</v>
       </c>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="23">
         <v>1200</v>
       </c>
-      <c r="C28" s="29">
+      <c r="C28" s="24">
         <f t="shared" si="0"/>
         <v>1221.5438889893928</v>
       </c>
-      <c r="D28" s="30">
+      <c r="D28" s="25">
         <f t="shared" si="1"/>
         <v>1285.9266942711251</v>
       </c>
-      <c r="E28" s="31">
+      <c r="E28" s="26">
         <v>1325.2232151426438</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="23">
         <v>1305.0210298984978</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="24">
         <v>1221.5438889893928</v>
       </c>
-      <c r="H28" s="30">
+      <c r="H28" s="25">
         <v>1285.9266942711251</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="26">
         <v>1312.0222384880924</v>
       </c>
-      <c r="J28" s="28">
+      <c r="J28" s="23">
         <v>1304.6306044805253</v>
       </c>
-      <c r="K28" s="29">
+      <c r="K28" s="24">
         <v>1292.7028952770554</v>
       </c>
-      <c r="L28" s="30">
+      <c r="L28" s="25">
         <v>1300.0522332826683</v>
       </c>
-      <c r="M28" s="31">
+      <c r="M28" s="26">
         <v>48.283561830002682</v>
       </c>
-      <c r="N28" s="32">
+      <c r="N28" s="27">
         <v>9.419985682308825</v>
       </c>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="4">
         <v>1300</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="6">
         <f t="shared" si="0"/>
         <v>1645.2269142658727</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="7">
         <f t="shared" si="1"/>
         <v>1609.652473298554</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="5">
         <v>1672.2122481837725</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="4">
         <v>1632.6963502501771</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="6">
         <v>1645.2269142658727</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="7">
         <v>1609.652473298554</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="5">
         <v>1656.8761430833451</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="4">
         <v>1619.6119469681989</v>
       </c>
-      <c r="K29" s="11">
+      <c r="K29" s="6">
         <v>1658.1761850099019</v>
       </c>
-      <c r="L29" s="12">
+      <c r="L29" s="7">
         <v>1620.3285694245535</v>
       </c>
-      <c r="M29" s="10">
+      <c r="M29" s="5">
         <v>7.8425767598033067</v>
       </c>
-      <c r="N29" s="8">
+      <c r="N29" s="3">
         <v>8.2349340843067367</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="34">
+      <c r="B30" s="29">
         <v>1400</v>
       </c>
-      <c r="C30" s="35">
+      <c r="C30" s="30">
         <f t="shared" si="0"/>
         <v>1711.4529004271042</v>
       </c>
-      <c r="D30" s="36">
+      <c r="D30" s="31">
         <f t="shared" si="1"/>
         <v>1666.2656028451881</v>
       </c>
-      <c r="E30" s="37">
+      <c r="E30" s="32">
         <v>1720.8820839104849</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30" s="29">
         <v>1700.0003867093733</v>
       </c>
-      <c r="G30" s="35">
+      <c r="G30" s="30">
         <v>1711.4529004271042</v>
       </c>
-      <c r="H30" s="36">
+      <c r="H30" s="31">
         <v>1666.2656028451881</v>
       </c>
-      <c r="I30" s="37">
+      <c r="I30" s="32">
         <v>1714.8586259069411</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="29">
         <v>1700.0001065044867</v>
       </c>
-      <c r="K30" s="35">
+      <c r="K30" s="30">
         <v>1715.5130590378678</v>
       </c>
-      <c r="L30" s="36">
+      <c r="L30" s="31">
         <v>1691.5665506408836</v>
       </c>
-      <c r="M30" s="37">
+      <c r="M30" s="32">
         <v>4.512685053557818</v>
       </c>
-      <c r="N30" s="38">
+      <c r="N30" s="33">
         <v>16.867298531195615</v>
       </c>
     </row>
@@ -2330,5 +2720,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>